<commit_message>
updates job suggestion results
</commit_message>
<xml_diff>
--- a/main/job_suggestions/candidate_1.xlsx
+++ b/main/job_suggestions/candidate_1.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -444,6 +444,11 @@
           <t>score</t>
         </is>
       </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>reason</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -452,7 +457,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>97</v>
+        <v>100</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+The job of NLP engineer remote is highly suitable for you as it requires the skills of NLP, Pytorch, Computer Vision, and Python, all of which you possess. The job also involves analyzing and preprocessing large-scale text data and developing prototypes, which aligns with your experience in LLMGuard and Literature Society IITJ Website projects. The high score of 100 indicates a strong match between your skills and the job requirements.</t>
+        </is>
       </c>
     </row>
     <row r="3">
@@ -462,7 +473,12 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>72</v>
+        <v>75</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>The job requires skills in MongoDB, ReactJS, JavaScript, Web Development, and NodeJS, which align with your experience and projects. The job offers the opportunity to work on high-quality web/mobile applications and suggests new features for product enhancement, which aligns with your skills in ReactJS and JavaScript. The job has a moderate score as it is a good fit for you, but there may be other candidates with more relevant experience.</t>
+        </is>
       </c>
     </row>
     <row r="4">
@@ -472,7 +488,13 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>69</v>
+        <v>62</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+The job has a moderate score of 62, indicating that it is neither highly suitable nor unsuitable for you. This is because the job requires skills in ReactJS, JavaScript, CSS, Frontend Development, and NextJS, which you have experience in through your projects. However, the job is an unpaid internship and for only 3 months, which may not be a good fit for your long-term career goals. </t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Removes langchain and updates requirements.txt
</commit_message>
<xml_diff>
--- a/main/job_suggestions/candidate_1.xlsx
+++ b/main/job_suggestions/candidate_1.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -457,43 +457,41 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-The job of NLP engineer remote is highly suitable for you as it requires the skills of NLP, Pytorch, Computer Vision, and Python, all of which you possess. The job also involves analyzing and preprocessing large-scale text data and developing prototypes, which aligns with your experience in LLMGuard and Literature Society IITJ Website projects. The high score of 100 indicates a strong match between your skills and the job requirements.</t>
+          <t>The job as an NLP engineer involves analyzing and preprocessing large-scale text data, and conducting PoCs in areas such as LLM, NLP, DL, ML, and object detection/classification. Your experience with projects like LLMGuard (bias detection), and Multi Model Data Analysis (data analysis) makes you well-suited for this role. Your skills in NLP, Pytorch, Computer Vision, and Python align closely with the required skills for this job, hence the high score of 97.</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>The job requires skills in MongoDB, ReactJS, JavaScript, Web Development, and NodeJS, which align with your experience and projects. The job offers the opportunity to work on high-quality web/mobile applications and suggests new features for product enhancement, which aligns with your skills in ReactJS and JavaScript. The job has a moderate score as it is a good fit for you, but there may be other candidates with more relevant experience.</t>
+          <t>The job of Frontend Engineer Intern is suitable for you because your experience in ReactJS, JavaScript, and CSS aligns well with the required skills for the job. Additionally, your projects involving ReactJS development make you a suitable candidate for ensuring efficient and visually appealing web design and user experience. The moderate score suggests that while you meet the basic requirements, there may be other factors influencing the hiring decision.</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-The job has a moderate score of 62, indicating that it is neither highly suitable nor unsuitable for you. This is because the job requires skills in ReactJS, JavaScript, CSS, Frontend Development, and NextJS, which you have experience in through your projects. However, the job is an unpaid internship and for only 3 months, which may not be a good fit for your long-term career goals. </t>
+          <t>The job of SDE Intern has a score of 71. This indicates that it is moderately suitable for you. The job requires skills such as MongoDB, ReactJS, JavaScript, Web Development, and NodeJS, which align with your experience in projects like LLMGuard and Literature Society IITJ Website. However, the job may not be a perfect fit as it may require additional skills or experience in certain areas.</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
integrates skill scoring for candidate assistance
</commit_message>
<xml_diff>
--- a/main/job_suggestions/candidate_1.xlsx
+++ b/main/job_suggestions/candidate_1.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,6 +446,11 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>reason</t>
         </is>
       </c>
@@ -457,26 +462,36 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>The job as an NLP engineer involves analyzing and preprocessing large-scale text data, and conducting PoCs in areas such as LLM, NLP, DL, ML, and object detection/classification. Your experience with projects like LLMGuard (bias detection), and Multi Model Data Analysis (data analysis) makes you well-suited for this role. Your skills in NLP, Pytorch, Computer Vision, and Python align closely with the required skills for this job, hence the high score of 97.</t>
+          <t>NLP Engineer (Remote): Collect and preprocess text corpora for language model training. Analyze data, develop and improve models. Skills: NLP, Pytorch, Computer Vision, Python.</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>The job of an NLP Engineer requires skills in NLP, Pytorch, Computer Vision, and Python. The candidate has experience in developing a pipeline for bias/toxicity detection in language models, utilizing GPT-2 and BERT, and implementing models for text analysis. The candidate's skills align well with the requirements of the job, making it suitable for the candidate.</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>4</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>71</v>
+        <v>41.5</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>The job of Frontend Engineer Intern is suitable for you because your experience in ReactJS, JavaScript, and CSS aligns well with the required skills for the job. Additionally, your projects involving ReactJS development make you a suitable candidate for ensuring efficient and visually appealing web design and user experience. The moderate score suggests that while you meet the basic requirements, there may be other factors influencing the hiring decision.</t>
+          <t>Application Development: Front-end coding for a sweat amino acid analysis app under a Scrum Master. Skills: Flutter, Dart, Android/iOS, Firestore, Firebase Authentication, Cloud Storage/Messaging, Mobile app architecture/design, Git.</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>The job involves front-end coding for a mobile app using Flutter and Dart, which aligns with your experience in ReactJS and JavaScript. The job also requires familiarity with mobile app architecture/design, which could be transferable skills from your previous projects. However, the job has a moderate score, suggesting that there may be other candidates with more relevant experience in Flutter and mobile app development.</t>
         </is>
       </c>
     </row>
@@ -487,11 +502,36 @@
         </is>
       </c>
       <c r="B4" t="n">
+        <v>75</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>SDE Intern: Remote MERN Stack Developer Internship, responsible for designing and developing web/mobile applications using MongoDB, ExpressJS, ReactJS, and NodeJS. Additional tasks include code maintenance, scalability, feature development, and product enhancement suggestions. Skills required: MongoDB, ReactJS, JavaScript, Web Development, NodeJS.</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>The job of a SDE Intern as a remote MERN Stack Developer requires skills in MongoDB, ReactJS, JavaScript, Web Development, and NodeJS. The candidate's experience in developing web applications using ReactJS, JavaScript, and their proficiency in MongoDB and NodeJS make them suitable for this role. The high score of 75.0 indicates a significant overlap between the job requirements and the candidate's skills.</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
         <v>71</v>
       </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>The job of SDE Intern has a score of 71. This indicates that it is moderately suitable for you. The job requires skills such as MongoDB, ReactJS, JavaScript, Web Development, and NodeJS, which align with your experience in projects like LLMGuard and Literature Society IITJ Website. However, the job may not be a perfect fit as it may require additional skills or experience in certain areas.</t>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Frontend Engineer Intern - Work in a team to ensure consistent web design and user experience, optimize web pages, and maintain brand consistency. Requires excellent communication skills and proficiency in ReactJS, JavaScript, CSS, and NextJS. 3-month evaluative unpaid internship with potential return offers.</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>The job as a Frontend Engineer Intern involves working in a team to maintain brand consistency and optimize web pages. Your experience in developing user-friendly UI using ReactJS and JavaScript makes you suitable. However, the unpaid nature of the internship and the evaluative period might be slight drawbacks. Overall, it appears to be a moderate fit for your skills and experience.</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
updates docstrings and comments in main files
</commit_message>
<xml_diff>
--- a/main/job_suggestions/candidate_1.xlsx
+++ b/main/job_suggestions/candidate_1.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,11 +446,6 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
           <t>reason</t>
         </is>
       </c>
@@ -462,56 +457,41 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>NLP Engineer (Remote): Collect and preprocess text corpora for language model training. Analyze data, develop and improve models. Skills: NLP, Pytorch, Computer Vision, Python.</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>The job of an NLP Engineer requires skills in NLP, Pytorch, Computer Vision, and Python. The candidate has experience in developing a pipeline for bias/toxicity detection in language models, utilizing GPT-2 and BERT, and implementing models for text analysis. The candidate's skills align well with the requirements of the job, making it suitable for the candidate.</t>
+          <t>The job of an NLP Engineer requires strong skills in NLP and Python, which you possess. Your experience in developing bias/toxicity detection pipelines and implementing language models aligns well with the job description. The high score indicates a strong match between your project experiences and the job requirements.</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>1</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>41.5</v>
+        <v>79</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Application Development: Front-end coding for a sweat amino acid analysis app under a Scrum Master. Skills: Flutter, Dart, Android/iOS, Firestore, Firebase Authentication, Cloud Storage/Messaging, Mobile app architecture/design, Git.</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>The job involves front-end coding for a mobile app using Flutter and Dart, which aligns with your experience in ReactJS and JavaScript. The job also requires familiarity with mobile app architecture/design, which could be transferable skills from your previous projects. However, the job has a moderate score, suggesting that there may be other candidates with more relevant experience in Flutter and mobile app development.</t>
+          <t>The job as a SDE Intern with a score of 79.0 is suitable for you because it requires skills in MongoDB, ReactJS, JavaScript, Web Development, and NodeJS. Your experience in developing web applications using ReactJS, MongoDB, and NodeJS aligns well with the job requirements. Additionally, your skillset in JavaScript and web development will be valuable for code maintenance, scalability, and feature development.</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>75</v>
+        <v>36.5</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>SDE Intern: Remote MERN Stack Developer Internship, responsible for designing and developing web/mobile applications using MongoDB, ExpressJS, ReactJS, and NodeJS. Additional tasks include code maintenance, scalability, feature development, and product enhancement suggestions. Skills required: MongoDB, ReactJS, JavaScript, Web Development, NodeJS.</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>The job of a SDE Intern as a remote MERN Stack Developer requires skills in MongoDB, ReactJS, JavaScript, Web Development, and NodeJS. The candidate's experience in developing web applications using ReactJS, JavaScript, and their proficiency in MongoDB and NodeJS make them suitable for this role. The high score of 75.0 indicates a significant overlap between the job requirements and the candidate's skills.</t>
+          <t>The job description of Application Development has a low score of 36.5. It is not suitable for you because it requires skills in Flutter, Dart, Android/iOS, Firestore, and Firebase Authentication which are not mentioned in your projects or resume.</t>
         </is>
       </c>
     </row>
@@ -522,16 +502,11 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Frontend Engineer Intern - Work in a team to ensure consistent web design and user experience, optimize web pages, and maintain brand consistency. Requires excellent communication skills and proficiency in ReactJS, JavaScript, CSS, and NextJS. 3-month evaluative unpaid internship with potential return offers.</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>The job as a Frontend Engineer Intern involves working in a team to maintain brand consistency and optimize web pages. Your experience in developing user-friendly UI using ReactJS and JavaScript makes you suitable. However, the unpaid nature of the internship and the evaluative period might be slight drawbacks. Overall, it appears to be a moderate fit for your skills and experience.</t>
+          <t>The job as a Frontend Engineer Intern requires proficiency in ReactJS, JavaScript, CSS, and NextJS, which aligns with your skills. The project 'LLMGuard' demonstrates your experience with ReactJS and JavaScript, making you suitable for this role. However, the unpaid evaluative internship and short duration may make it less desirable compared to other options.</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
resolves bug in candAssistant
</commit_message>
<xml_diff>
--- a/main/job_suggestions/candidate_1.xlsx
+++ b/main/job_suggestions/candidate_1.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -457,11 +457,11 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>The job of an NLP Engineer requires strong skills in NLP and Python, which you possess. Your experience in developing bias/toxicity detection pipelines and implementing language models aligns well with the job description. The high score indicates a strong match between your project experiences and the job requirements.</t>
+          <t>The job of NLP Engineer is highly suitable for you as it aligns perfectly with your experience in developing bias/toxicity detection pipelines for language models and utilizing PyTorch and Python in your projects. Your skills in NLP, PyTorch, and Python make you a strong fit for this role.</t>
         </is>
       </c>
     </row>
@@ -472,41 +472,28 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>The job as a SDE Intern with a score of 79.0 is suitable for you because it requires skills in MongoDB, ReactJS, JavaScript, Web Development, and NodeJS. Your experience in developing web applications using ReactJS, MongoDB, and NodeJS aligns well with the job requirements. Additionally, your skillset in JavaScript and web development will be valuable for code maintenance, scalability, and feature development.</t>
+          <t>**Job Description:** SDE Intern: Remote MERN Stack Developer Internship, responsible for designing and developing web/mobile applications using MongoDB, ExpressJS, ReactJS, and NodeJS. Additional tasks include code maintenance, scalability, feature development, and product enhancement suggestions. Skills required: MongoDB, ReactJS, JavaScript, Web Development, NodeJS.
+**Score:** 77
+**Reasoning:** The job as a MERN Stack Developer Intern is suitable due to the candidate's experience with ReactJS, Python, and JavaScript, aligning well with the required skills. The candidate's proficiency in developing web applications makes them a good fit for tasks related to feature development and product enhancement.</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>2</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>36.5</v>
+        <v>68</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>The job description of Application Development has a low score of 36.5. It is not suitable for you because it requires skills in Flutter, Dart, Android/iOS, Firestore, and Firebase Authentication which are not mentioned in your projects or resume.</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>70</v>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>The job as a Frontend Engineer Intern requires proficiency in ReactJS, JavaScript, CSS, and NextJS, which aligns with your skills. The project 'LLMGuard' demonstrates your experience with ReactJS and JavaScript, making you suitable for this role. However, the unpaid evaluative internship and short duration may make it less desirable compared to other options.</t>
+          <t>The Frontend Engineer Intern position is moderately suitable for you based on your experience with ReactJS and JavaScript. It aligns well with your skills in web development and offers an opportunity to enhance your frontend expertise during the internship period.</t>
         </is>
       </c>
     </row>

</xml_diff>